<commit_message>
fix elocationid and language
</commit_message>
<xml_diff>
--- a/Transformed_PubMed_Data.xlsx
+++ b/Transformed_PubMed_Data.xlsx
@@ -829,7 +829,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>eng</t>
+          <t>{eng}</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>{pii: S0161-6420(20)31043-5}</t>
+          <t>{pii: S0161-6420(20)31043-5||doi: 10.1016/j.ophtha.2020.10.040}</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>eng</t>
+          <t>{eng||spa}</t>
         </is>
       </c>
       <c r="X4" t="inlineStr"/>

</xml_diff>

<commit_message>
Added multiple Author and Grant list
</commit_message>
<xml_diff>
--- a/Transformed_PubMed_Data.xlsx
+++ b/Transformed_PubMed_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
   <si>
     <t>Order</t>
   </si>
@@ -82,12 +82,21 @@
     <t>AuthorList</t>
   </si>
   <si>
+    <t>AuthorList_Fullnames</t>
+  </si>
+  <si>
+    <t>AuthorList_Abbreviated</t>
+  </si>
+  <si>
     <t>Language</t>
   </si>
   <si>
     <t>GrantList</t>
   </si>
   <si>
+    <t>Grant_Number</t>
+  </si>
+  <si>
     <t>PublicationTypeList</t>
   </si>
   <si>
@@ -130,6 +139,12 @@
     <t>PersonalNameSubjectList</t>
   </si>
   <si>
+    <t>PersonalNameSubjectList_Fullnames</t>
+  </si>
+  <si>
+    <t>PersonalNameSubjectList_Abbreviated</t>
+  </si>
+  <si>
     <t>OtherID</t>
   </si>
   <si>
@@ -148,6 +163,12 @@
     <t>InvestigatorList</t>
   </si>
   <si>
+    <t>InvestigatorList_Fullnames</t>
+  </si>
+  <si>
+    <t>InvestigatorList_Abbreviated</t>
+  </si>
+  <si>
     <t>GeneralNote</t>
   </si>
   <si>
@@ -280,10 +301,22 @@
     <t>Copyright © 2020 American Academy of Ophthalmology. Published by Elsevier Inc. All rights reserved.</t>
   </si>
   <si>
-    <t>{Position: 1||LastName: Hiruma||ForeName: Laura||Initials: L||ORCID: http://orcid.org/0000-0003-4192-4376 ||Affiliation 1: test1||Affiliation 2: test2}, {Position: 2||LastName: Pretzel||ForeName: Rebecca Edmondson||Initials: RE||Suffix: Jr||Affiliation 1: Carolina Institute for Developmental Disabilities, University of North Carolina at Chapel Hill, Campus Box #7255, Chapel Hill, NC, 27599-7255, USA.}, {Position: 3||LastName: Tapia||ForeName: Amanda||Initials: A||Affiliation 1: Department of Biostatistics, Collaborative Studies Coordinating Center, University of North Carolina at Chapel Hill, Campus Box #8030, Chapel Hill, NC, 27516, USA.}, {Position: 4||CollectiveName: OPAL Collective}</t>
-  </si>
-  <si>
-    <t>{Position: 1||LastName: Modjtahedi||ForeName: Bobeck S||Initials: BS||Affiliation 1: Department of Ophthalmology, Southern California Kaiser Permanente, Baldwin Park, California; Department of Research and Evaluation, Southern California Permanente Medical Group, Pasadena, California.}, {Position: 2||LastName: Abbott||ForeName: Richard L||Initials: RL||Affiliation 1: Department of Ophthalmology, University of California, San Francisco, San Francisco, California.}, {Position: 3||LastName: Fong||ForeName: Donald S||Initials: DS||Affiliation 1: Department of Ophthalmology, Southern California Kaiser Permanente, Baldwin Park, California; Department of Research and Evaluation, Southern California Permanente Medical Group, Pasadena, California.}, {Position: 4||LastName: Lum||ForeName: Flora||Initials: F||Affiliation 1: American Academy of Ophthalmology, San Francisco, California. Electronic address: flum@aao.org.}, {Position: 5||LastName: Tan||ForeName: Donald||Initials: D||Affiliation 1: Eye and Retina Surgeons, Singapore, Republic of Singapore.}, {Position: 6||CollectiveName: Task Force on Myopia}</t>
+    <t>Position: 1\LastName: Hiruma\ForeName: Laura\Initials: L\ORCID: http://orcid.org/0000-0003-4192-4376/\Affiliation 1: test1\Affiliation 2: test2||Position: 2\LastName: Pretzel\ForeName: Rebecca Edmondson\Initials: RE\Suffix: Jr\Affiliation 1: Carolina Institute for Developmental Disabilities, University of North Carolina at Chapel Hill, Campus Box #7255, Chapel Hill, NC, 27599-7255, USA.||Position: 3\LastName: Tapia\ForeName: Amanda\Initials: A\Affiliation 1: Department of Biostatistics, Collaborative Studies Coordinating Center, University of North Carolina at Chapel Hill, Campus Box #8030, Chapel Hill, NC, 27516, USA.||Position: 4\CollectiveName: OPAL Collective</t>
+  </si>
+  <si>
+    <t>Position: 1\LastName: Modjtahedi\ForeName: Bobeck S\Initials: BS\Affiliation 1: Department of Ophthalmology, Southern California Kaiser Permanente, Baldwin Park, California; Department of Research and Evaluation, Southern California Permanente Medical Group, Pasadena, California.||Position: 2\LastName: Abbott\ForeName: Richard L\Initials: RL\Affiliation 1: Department of Ophthalmology, University of California, San Francisco, San Francisco, California.||Position: 3\LastName: Fong\ForeName: Donald S\Initials: DS\Affiliation 1: Department of Ophthalmology, Southern California Kaiser Permanente, Baldwin Park, California; Department of Research and Evaluation, Southern California Permanente Medical Group, Pasadena, California.||Position: 4\LastName: Lum\ForeName: Flora\Initials: F\Affiliation 1: American Academy of Ophthalmology, San Francisco, California. Electronic address: flum@aao.org.||Position: 5\LastName: Tan\ForeName: Donald\Initials: D\Affiliation 1: Eye and Retina Surgeons, Singapore, Republic of Singapore.||Position: 6\CollectiveName: Task Force on Myopia</t>
+  </si>
+  <si>
+    <t>Hiruma, Laura||Pretzel, Rebecca Edmondson Jr||Tapia, Amanda||OPAL Collective</t>
+  </si>
+  <si>
+    <t>Modjtahedi, Bobeck S||Abbott, Richard L||Fong, Donald S||Lum, Flora||Tan, Donald||Task Force on Myopia</t>
+  </si>
+  <si>
+    <t>Hiruma L||Pretzel RE||Tapia A||OPAL Collective</t>
+  </si>
+  <si>
+    <t>Modjtahedi BS||Abbott RL||Fong DS||Lum F||Tan D||Task Force on Myopia</t>
   </si>
   <si>
     <t>{eng}</t>
@@ -295,6 +328,9 @@
     <t>{Position: 1||GrantID: U10 DD000180||Acronym: DD||Agency: NCBDD CDC HHS||Country: United States}, {Position: 2||GrantID: CC999999||Acronym: ImCDC||Agency: Intramural CDC HHS||Country: United States}, {Position: 3||GrantID: U10 DD000183||Acronym: DD||Agency: NCBDD CDC HHS||Country: United States}</t>
   </si>
   <si>
+    <t>U10 DD000180\DD\NCBDD CDC HHS\United States||CC999999\ImCDC\Intramural CDC HHS\United States||U10 DD000183\DD\NCBDD CDC HHS\United States</t>
+  </si>
+  <si>
     <t>{PublicationType: Journal Article||UI: D016428}</t>
   </si>
   <si>
@@ -343,7 +379,13 @@
     <t>38</t>
   </si>
   <si>
-    <t>{Position: 1||LastName: Darwin||ForeName: Charles||Initials: C}, {Position: 2||LastName: Hume||ForeName: David||Initials: D}, {Position: 3||LastName: Morgan||ForeName: C Lloyd||Initials: CL}</t>
+    <t>Position: 1\LastName: Darwin\ForeName: Charles\Initials: C||Position: 2\LastName: Hume\ForeName: David\Initials: D||Position: 3\LastName: Morgan\ForeName: C Lloyd\Initials: CL</t>
+  </si>
+  <si>
+    <t>Darwin, Charles||Hume, David||Morgan, C Lloyd</t>
+  </si>
+  <si>
+    <t>Darwin C||Hume D||Morgan CL</t>
   </si>
   <si>
     <t>{OtherID: 00022554||Source: NASA}</t>
@@ -364,10 +406,22 @@
     <t>{SpaceFlightMission: Flight Experiment}||{SpaceFlightMission: STS-55 Shuttle Project}||{SpaceFlightMission: manned}||{SpaceFlightMission: short duration}</t>
   </si>
   <si>
-    <t>{Position: 1||LastName: Carlsson||ForeName: Christer||Initials: C||ORCID: http://orcid.org/0000-0003-4192-4376 ||Affiliation 1: test1||Affiliation 2: test2}, {Position: 2||LastName: Cecchi||ForeName: Francesca||Initials: F}</t>
-  </si>
-  <si>
-    <t>{Position: 1||LastName: Ang||ForeName: Marcus||Initials: M}, {Position: 2||LastName: Chiarito||ForeName: Susan||Initials: S}, {Position: 3||LastName: Cotter||ForeName: Susan A||Initials: SA}, {Position: 4||LastName: Fernandez||ForeName: Angela Maria||Initials: AM}, {Position: 5||LastName: Grzybowski||ForeName: Andrzej||Initials: A}, {Position: 6||LastName: He||ForeName: Mingguang||Initials: M}, {Position: 7||LastName: Jacobs||ForeName: Deborah S||Initials: DS}, {Position: 8||LastName: Jonas||ForeName: Jost B||Initials: JB}, {Position: 9||LastName: Kemper||ForeName: Alex||Initials: A}, {Position: 10||LastName: Lee||ForeName: Katherine A||Initials: KA}, {Position: 11||LastName: Molinari||ForeName: Andrea Delia||Initials: AD}, {Position: 12||LastName: Morgan||ForeName: Ian||Initials: I}, {Position: 13||LastName: Ohno-Matsui||ForeName: Kyoko||Initials: K}, {Position: 14||LastName: Repka||ForeName: Michael X||Initials: MX}, {Position: 15||LastName: Salim||ForeName: Sarwat||Initials: S}, {Position: 16||LastName: Wu||ForeName: Pei-Chang||Initials: PC}, {Position: 17||LastName: Yao||ForeName: Ke||Initials: K}, {Position: 18||LastName: Zadnik||ForeName: Karla||Initials: K}</t>
+    <t>Position: 1\LastName: Carlsson\ForeName: Christer\Initials: C\ORCID: http://orcid.org/0000-0003-4192-4376/\Affiliation 1: test1\Affiliation 2: test2||Position: 2\LastName: Cecchi\ForeName: Francesca\Initials: F</t>
+  </si>
+  <si>
+    <t>Position: 1\LastName: Ang\ForeName: Marcus\Initials: M||Position: 2\LastName: Chiarito\ForeName: Susan\Initials: S||Position: 3\LastName: Cotter\ForeName: Susan A\Initials: SA||Position: 4\LastName: Fernandez\ForeName: Angela Maria\Initials: AM||Position: 5\LastName: Grzybowski\ForeName: Andrzej\Initials: A||Position: 6\LastName: He\ForeName: Mingguang\Initials: M||Position: 7\LastName: Jacobs\ForeName: Deborah S\Initials: DS||Position: 8\LastName: Jonas\ForeName: Jost B\Initials: JB||Position: 9\LastName: Kemper\ForeName: Alex\Initials: A||Position: 10\LastName: Lee\ForeName: Katherine A\Initials: KA||Position: 11\LastName: Molinari\ForeName: Andrea Delia\Initials: AD||Position: 12\LastName: Morgan\ForeName: Ian\Initials: I||Position: 13\LastName: Ohno-Matsui\ForeName: Kyoko\Initials: K||Position: 14\LastName: Repka\ForeName: Michael X\Initials: MX||Position: 15\LastName: Salim\ForeName: Sarwat\Initials: S||Position: 16\LastName: Wu\ForeName: Pei-Chang\Initials: PC||Position: 17\LastName: Yao\ForeName: Ke\Initials: K||Position: 18\LastName: Zadnik\ForeName: Karla\Initials: K</t>
+  </si>
+  <si>
+    <t>Carlsson, Christer||Cecchi, Francesca</t>
+  </si>
+  <si>
+    <t>Ang, Marcus||Chiarito, Susan||Cotter, Susan A||Fernandez, Angela Maria||Grzybowski, Andrzej||He, Mingguang||Jacobs, Deborah S||Jonas, Jost B||Kemper, Alex||Lee, Katherine A||Molinari, Andrea Delia||Morgan, Ian||Ohno-Matsui, Kyoko||Repka, Michael X||Salim, Sarwat||Wu, Pei-Chang||Yao, Ke||Zadnik, Karla</t>
+  </si>
+  <si>
+    <t>Carlsson C||Cecchi F</t>
+  </si>
+  <si>
+    <t>Ang M||Chiarito S||Cotter SA||Fernandez AM||Grzybowski A||He M||Jacobs DS||Jonas JB||Kemper A||Lee KA||Molinari AD||Morgan I||Ohno-Matsui K||Repka MX||Salim S||Wu PC||Yao K||Zadnik K</t>
   </si>
   <si>
     <t>{Owner: KIE||GeneralNote: 38 refs.}</t>
@@ -762,13 +816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF5"/>
+  <dimension ref="A1:BM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,25 +997,46 @@
       <c r="BF1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:65">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G2" s="2">
         <v>44466</v>
@@ -970,170 +1045,191 @@
         <v>44470</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="M2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="N2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="O2" s="2">
         <v>44197</v>
       </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="R2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="S2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="T2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="U2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="V2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="W2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="X2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="Y2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z2" s="2">
+        <v>101</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC2" s="2">
         <v>44198</v>
       </c>
-      <c r="AA2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>97</v>
-      </c>
       <c r="AD2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="AE2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="AF2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="AG2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="AH2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="AI2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="AJ2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="AK2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AL2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AM2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AN2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="AO2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="AP2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="AQ2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="AR2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="AS2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AT2" s="2">
+        <v>125</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>136</v>
+      </c>
+      <c r="BA2" s="2">
         <v>44133</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="BB2" s="2">
         <v>44199</v>
       </c>
-      <c r="AV2" s="2">
+      <c r="BC2" s="2">
         <v>44467</v>
       </c>
-      <c r="AW2" s="2">
+      <c r="BD2" s="2">
         <v>44198</v>
       </c>
-      <c r="AX2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>122</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>123</v>
-      </c>
       <c r="BE2" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="BF2" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:65">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>127</v>
+        <v>70</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:65">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G4" s="2">
         <v>44481</v>
@@ -1142,114 +1238,126 @@
         <v>44481</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="O4" s="2">
         <v>40909</v>
       </c>
       <c r="P4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="R4" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="S4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="T4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="U4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="V4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="W4" t="s">
-        <v>91</v>
+        <v>98</v>
+      </c>
+      <c r="X4" t="s">
+        <v>100</v>
       </c>
       <c r="Y4" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z4" s="2">
+        <v>102</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC4" s="2">
         <v>41299</v>
       </c>
-      <c r="AA4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>98</v>
-      </c>
       <c r="AD4" t="s">
-        <v>100</v>
+        <v>107</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>110</v>
       </c>
       <c r="AG4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="AJ4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT4" s="2">
+        <v>115</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA4" s="2">
         <v>44133</v>
       </c>
-      <c r="AU4" s="2">
+      <c r="BB4" s="2">
         <v>44200</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="BC4" s="2">
         <v>44482</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="BD4" s="2">
         <v>44199</v>
       </c>
-      <c r="AX4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC4" s="2">
+      <c r="BE4" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>139</v>
+      </c>
+      <c r="BJ4" s="2">
         <v>44123</v>
       </c>
-      <c r="BD4" s="2">
+      <c r="BK4" s="2">
         <v>44131</v>
       </c>
-      <c r="BE4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>128</v>
+      <c r="BL4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:65">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>127</v>
+        <v>70</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>